<commit_message>
pemisahan export dan print
</commit_message>
<xml_diff>
--- a/assets/excel/Report Bezetting.xlsx
+++ b/assets/excel/Report Bezetting.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="282">
   <si>
     <t>REPORT BEZETTING</t>
   </si>
@@ -41,7 +41,7 @@
     <t>Ket.</t>
   </si>
   <si>
-    <t>Abdul Latief Baedhowi/Palembang/1982-06-08</t>
+    <t>Abdul Latief Baedhowi//</t>
   </si>
   <si>
     <t>2012.12.01.002</t>
@@ -50,111 +50,111 @@
     <t>Direktur Operasional</t>
   </si>
   <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>Aktif</t>
+  </si>
+  <si>
+    <t>Ahmad Hanif//</t>
+  </si>
+  <si>
+    <t>2012.12.01.003</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>Iwan Setiyawan/Bantul/2022-06-06</t>
+  </si>
+  <si>
+    <t>2012.12.01.004</t>
+  </si>
+  <si>
+    <t>Tri Wardaningtyas//</t>
+  </si>
+  <si>
+    <t>2012.12.01.005</t>
+  </si>
+  <si>
+    <t>Sudarsono//</t>
+  </si>
+  <si>
+    <t>2012.12.01.006</t>
+  </si>
+  <si>
+    <t>Tri Bekti Rianto//</t>
+  </si>
+  <si>
+    <t>2012.12.01.008</t>
+  </si>
+  <si>
+    <t>Samiran//</t>
+  </si>
+  <si>
+    <t>2012.12.01.009</t>
+  </si>
+  <si>
+    <t>SMP</t>
+  </si>
+  <si>
+    <t>Edy Rusmanto//</t>
+  </si>
+  <si>
+    <t>2012.12.01.010</t>
+  </si>
+  <si>
+    <t>SMK</t>
+  </si>
+  <si>
+    <t>Roni Slamet//</t>
+  </si>
+  <si>
+    <t>2012.12.01.011</t>
+  </si>
+  <si>
+    <t>DIII</t>
+  </si>
+  <si>
+    <t>Ihsanuddin//</t>
+  </si>
+  <si>
+    <t>2012.12.01.012</t>
+  </si>
+  <si>
+    <t>Sukirman//</t>
+  </si>
+  <si>
+    <t>2012.12.01.013</t>
+  </si>
+  <si>
+    <t>Bambang Gunartok//</t>
+  </si>
+  <si>
+    <t>2012.12.01.014</t>
+  </si>
+  <si>
+    <t>Rudi Riswanto//</t>
+  </si>
+  <si>
+    <t>2012.12.01.015</t>
+  </si>
+  <si>
+    <t>Maryono//</t>
+  </si>
+  <si>
+    <t>2012.12.01.016</t>
+  </si>
+  <si>
+    <t>Muryanto//</t>
+  </si>
+  <si>
+    <t>2012.12.01.017</t>
+  </si>
+  <si>
     <t>SMA</t>
   </si>
   <si>
-    <t>Aktif</t>
-  </si>
-  <si>
-    <t>Ahmad Hanif//</t>
-  </si>
-  <si>
-    <t>2012.12.01.003</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>Iwan Setiyawan//</t>
-  </si>
-  <si>
-    <t>2012.12.01.004</t>
-  </si>
-  <si>
-    <t>Tri Wardaningtyas//</t>
-  </si>
-  <si>
-    <t>2012.12.01.005</t>
-  </si>
-  <si>
-    <t>Sudarsono//</t>
-  </si>
-  <si>
-    <t>2012.12.01.006</t>
-  </si>
-  <si>
-    <t>Tri Bekti Rianto//</t>
-  </si>
-  <si>
-    <t>2012.12.01.008</t>
-  </si>
-  <si>
-    <t>Samiran//</t>
-  </si>
-  <si>
-    <t>2012.12.01.009</t>
-  </si>
-  <si>
-    <t>SMP</t>
-  </si>
-  <si>
-    <t>Edy Rusmanto//</t>
-  </si>
-  <si>
-    <t>2012.12.01.010</t>
-  </si>
-  <si>
-    <t>SMK</t>
-  </si>
-  <si>
-    <t>Roni Slamet//</t>
-  </si>
-  <si>
-    <t>2012.12.01.011</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>Ihsanuddin//</t>
-  </si>
-  <si>
-    <t>2012.12.01.012</t>
-  </si>
-  <si>
-    <t>Sukirman//</t>
-  </si>
-  <si>
-    <t>2012.12.01.013</t>
-  </si>
-  <si>
-    <t>Bambang Gunartok//</t>
-  </si>
-  <si>
-    <t>2012.12.01.014</t>
-  </si>
-  <si>
-    <t>Rudi Riswanto//</t>
-  </si>
-  <si>
-    <t>2012.12.01.015</t>
-  </si>
-  <si>
-    <t>Maryono//</t>
-  </si>
-  <si>
-    <t>2012.12.01.016</t>
-  </si>
-  <si>
-    <t>Muryanto//</t>
-  </si>
-  <si>
-    <t>2012.12.01.017</t>
-  </si>
-  <si>
     <t>Heri Susanto//</t>
   </si>
   <si>
@@ -855,6 +855,9 @@
   </si>
   <si>
     <t>Burhanu Sultan Ramadan/Darit/2001-08-09</t>
+  </si>
+  <si>
+    <t>Staff</t>
   </si>
   <si>
     <t>ratnasari/Darit/2001-08-09</t>
@@ -1246,7 +1249,7 @@
         <v>11</v>
       </c>
       <c r="F4">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="G4" t="s">
         <v>12</v>
@@ -1262,11 +1265,9 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5"/>
+      <c r="E5" t="s">
         <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1280,13 +1281,15 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
       <c r="D6"/>
-      <c r="E6"/>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
       <c r="F6">
         <v>0</v>
       </c>
@@ -1299,14 +1302,14 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
       </c>
       <c r="D7"/>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1320,14 +1323,14 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
         <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
       </c>
       <c r="D8"/>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1341,10 +1344,10 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
         <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
       </c>
       <c r="D9"/>
       <c r="E9"/>
@@ -1360,14 +1363,14 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
         <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
       </c>
       <c r="D10"/>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1381,14 +1384,14 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
         <v>28</v>
-      </c>
-      <c r="C11" t="s">
-        <v>29</v>
       </c>
       <c r="D11"/>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1402,14 +1405,14 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
         <v>31</v>
-      </c>
-      <c r="C12" t="s">
-        <v>32</v>
       </c>
       <c r="D12"/>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1423,14 +1426,14 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
         <v>34</v>
-      </c>
-      <c r="C13" t="s">
-        <v>35</v>
       </c>
       <c r="D13"/>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1444,10 +1447,10 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
         <v>36</v>
-      </c>
-      <c r="C14" t="s">
-        <v>37</v>
       </c>
       <c r="D14"/>
       <c r="E14"/>
@@ -1463,14 +1466,14 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
         <v>38</v>
-      </c>
-      <c r="C15" t="s">
-        <v>39</v>
       </c>
       <c r="D15"/>
       <c r="E15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1484,14 +1487,14 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
         <v>40</v>
-      </c>
-      <c r="C16" t="s">
-        <v>41</v>
       </c>
       <c r="D16"/>
       <c r="E16" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1505,14 +1508,14 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
         <v>42</v>
-      </c>
-      <c r="C17" t="s">
-        <v>43</v>
       </c>
       <c r="D17"/>
       <c r="E17" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1526,14 +1529,14 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
         <v>44</v>
-      </c>
-      <c r="C18" t="s">
-        <v>45</v>
       </c>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -1572,7 +1575,9 @@
         <v>49</v>
       </c>
       <c r="D20"/>
-      <c r="E20"/>
+      <c r="E20" t="s">
+        <v>32</v>
+      </c>
       <c r="F20">
         <v>0</v>
       </c>
@@ -1781,7 +1786,9 @@
         <v>71</v>
       </c>
       <c r="D31"/>
-      <c r="E31"/>
+      <c r="E31" t="s">
+        <v>11</v>
+      </c>
       <c r="F31">
         <v>0</v>
       </c>
@@ -3954,7 +3961,9 @@
       <c r="D148" t="s">
         <v>260</v>
       </c>
-      <c r="E148"/>
+      <c r="E148" t="s">
+        <v>32</v>
+      </c>
       <c r="F148">
         <v>0</v>
       </c>
@@ -4295,7 +4304,9 @@
       <c r="C168">
         <v>123</v>
       </c>
-      <c r="D168"/>
+      <c r="D168" t="s">
+        <v>280</v>
+      </c>
       <c r="E168"/>
       <c r="F168">
         <v>20</v>
@@ -4309,7 +4320,7 @@
         <v>166</v>
       </c>
       <c r="B169" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C169">
         <v>1234</v>

</xml_diff>

<commit_message>
menghapus file file dan perbaikan
</commit_message>
<xml_diff>
--- a/assets/excel/Report Bezetting.xlsx
+++ b/assets/excel/Report Bezetting.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="275">
   <si>
     <t>REPORT BEZETTING</t>
   </si>
@@ -834,6 +834,12 @@
   </si>
   <si>
     <t>Burhanu Sultan Ramadan/Darit/2001-08-09</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>S3</t>
   </si>
 </sst>
 </file>
@@ -4243,8 +4249,12 @@
       <c r="C168">
         <v>9535253</v>
       </c>
-      <c r="D168"/>
-      <c r="E168"/>
+      <c r="D168" t="s">
+        <v>273</v>
+      </c>
+      <c r="E168" t="s">
+        <v>274</v>
+      </c>
       <c r="F168">
         <v>20</v>
       </c>

</xml_diff>